<commit_message>
filtration by search string, group and subgroup implemented"
</commit_message>
<xml_diff>
--- a/docs/assets/excel/dictionary.xlsx
+++ b/docs/assets/excel/dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="Workbook_______" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/448a1b2199d98c32/Рабочий стол/Університет/Darina/dictionary/src/assets/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ДИПЛОМ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{178C9F5B-CEF2-4EB8-919F-5E8BECB8F957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3DFEA1-95B2-403F-80E4-1D89C19443E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -7211,27 +7211,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Worksheet_____1"/>
-  <dimension ref="A1:H204"/>
+  <dimension ref="A1:I204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E204" sqref="E204"/>
+    <sheetView tabSelected="1" topLeftCell="E154" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.6328125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.81640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="102.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.90625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="60.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="60.453125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.90625" style="6"/>
+    <col min="3" max="3" width="57.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="102.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.88671875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="60.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="60.44140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>704</v>
       </c>
@@ -7257,7 +7257,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -7282,8 +7282,11 @@
       <c r="H2" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -7308,8 +7311,11 @@
       <c r="H3" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="131.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="131.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>495</v>
       </c>
@@ -7331,8 +7337,11 @@
       <c r="G4" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.35">
+      <c r="I4" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -7357,8 +7366,11 @@
       <c r="H5" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I5" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -7383,8 +7395,11 @@
       <c r="H6" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.35">
+      <c r="I6" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="108" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -7406,8 +7421,11 @@
       <c r="G7" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I7" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>478</v>
       </c>
@@ -7429,8 +7447,11 @@
       <c r="G8" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I8" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>381</v>
       </c>
@@ -7452,8 +7473,11 @@
       <c r="G9" s="4" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.35">
+      <c r="I9" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
@@ -7478,8 +7502,11 @@
       <c r="H10" s="4" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I10" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>380</v>
       </c>
@@ -7504,8 +7531,11 @@
       <c r="H11" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I11" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>369</v>
       </c>
@@ -7530,8 +7560,11 @@
       <c r="H12" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I12" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -7553,8 +7586,11 @@
       <c r="G13" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I13" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>480</v>
       </c>
@@ -7576,8 +7612,11 @@
       <c r="G14" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.35">
+      <c r="I14" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="90" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -7602,8 +7641,11 @@
       <c r="H15" s="4" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I15" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>448</v>
       </c>
@@ -7628,8 +7670,11 @@
       <c r="H16" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I16" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -7654,8 +7699,11 @@
       <c r="H17" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I17" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -7680,8 +7728,11 @@
       <c r="H18" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I18" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>237</v>
       </c>
@@ -7703,8 +7754,11 @@
       <c r="G19" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I19" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>386</v>
       </c>
@@ -7726,8 +7780,11 @@
       <c r="G20" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>522</v>
       </c>
@@ -7752,8 +7809,11 @@
       <c r="H21" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I21" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>560</v>
       </c>
@@ -7778,8 +7838,11 @@
       <c r="H22" s="4" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="75.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>528</v>
       </c>
@@ -7804,8 +7867,11 @@
       <c r="H23" s="4" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I23" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>375</v>
       </c>
@@ -7830,8 +7896,11 @@
       <c r="H24" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I24" s="6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>536</v>
       </c>
@@ -7856,8 +7925,11 @@
       <c r="H25" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I25" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>443</v>
       </c>
@@ -7882,8 +7954,11 @@
       <c r="H26" s="4" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I26" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>388</v>
       </c>
@@ -7905,8 +7980,11 @@
       <c r="G27" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I27" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
@@ -7928,8 +8006,11 @@
       <c r="G28" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I28" s="6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>397</v>
       </c>
@@ -7954,8 +8035,11 @@
       <c r="H29" s="4" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I29" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>402</v>
       </c>
@@ -7980,8 +8064,11 @@
       <c r="H30" s="4" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I30" s="6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>481</v>
       </c>
@@ -8006,8 +8093,11 @@
       <c r="H31" s="4" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I31" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>419</v>
       </c>
@@ -8032,8 +8122,11 @@
       <c r="H32" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I32" s="6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>228</v>
       </c>
@@ -8058,8 +8151,11 @@
       <c r="H33" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="90" x14ac:dyDescent="0.35">
+      <c r="I33" s="6">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="90" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>389</v>
       </c>
@@ -8084,8 +8180,11 @@
       <c r="H34" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I34" s="6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>246</v>
       </c>
@@ -8110,8 +8209,11 @@
       <c r="H35" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I35" s="6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>249</v>
       </c>
@@ -8133,8 +8235,11 @@
       <c r="G36" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="I36" s="6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>463</v>
       </c>
@@ -8159,8 +8264,11 @@
       <c r="H37" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I37" s="6">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>566</v>
       </c>
@@ -8185,8 +8293,11 @@
       <c r="H38" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38" s="6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>20</v>
       </c>
@@ -8211,8 +8322,11 @@
       <c r="H39" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I39" s="6">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>541</v>
       </c>
@@ -8234,8 +8348,11 @@
       <c r="G40" s="4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I40" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>414</v>
       </c>
@@ -8257,8 +8374,11 @@
       <c r="G41" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I41" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>342</v>
       </c>
@@ -8283,8 +8403,11 @@
       <c r="H42" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I42" s="6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>21</v>
       </c>
@@ -8309,8 +8432,11 @@
       <c r="H43" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I43" s="6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>22</v>
       </c>
@@ -8335,8 +8461,11 @@
       <c r="H44" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I44" s="6">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>41</v>
       </c>
@@ -8358,8 +8487,11 @@
       <c r="G45" s="4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I45" s="6">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>42</v>
       </c>
@@ -8381,8 +8513,11 @@
       <c r="G46" s="4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I46" s="6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>768</v>
       </c>
@@ -8407,8 +8542,11 @@
       <c r="H47" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I47" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>238</v>
       </c>
@@ -8430,8 +8568,11 @@
       <c r="G48" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I48" s="6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>43</v>
       </c>
@@ -8456,8 +8597,11 @@
       <c r="H49" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I49" s="6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>44</v>
       </c>
@@ -8482,8 +8626,11 @@
       <c r="H50" s="4" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.35">
+      <c r="I50" s="6">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>241</v>
       </c>
@@ -8508,8 +8655,11 @@
       <c r="H51" s="4" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I51" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>49</v>
       </c>
@@ -8534,8 +8684,11 @@
       <c r="H52" s="4" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I52" s="6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>403</v>
       </c>
@@ -8560,8 +8713,11 @@
       <c r="H53" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I53" s="6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>406</v>
       </c>
@@ -8586,8 +8742,11 @@
       <c r="H54" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I54" s="6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>492</v>
       </c>
@@ -8609,8 +8768,11 @@
       <c r="G55" s="4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="I55" s="6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>50</v>
       </c>
@@ -8635,8 +8797,11 @@
       <c r="H56" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I56" s="6">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>51</v>
       </c>
@@ -8658,8 +8823,11 @@
       <c r="G57" s="4" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I57" s="6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>52</v>
       </c>
@@ -8681,8 +8849,11 @@
       <c r="G58" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I58" s="6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>543</v>
       </c>
@@ -8707,8 +8878,11 @@
       <c r="H59" s="4" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I59" s="6">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>53</v>
       </c>
@@ -8730,8 +8904,11 @@
       <c r="G60" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I60" s="6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>507</v>
       </c>
@@ -8753,8 +8930,11 @@
       <c r="G61" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I61" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>415</v>
       </c>
@@ -8779,8 +8959,11 @@
       <c r="H62" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I62" s="6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>338</v>
       </c>
@@ -8802,8 +8985,11 @@
       <c r="G63" s="4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I63" s="6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>54</v>
       </c>
@@ -8828,8 +9014,11 @@
       <c r="H64" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I64" s="6">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>48</v>
       </c>
@@ -8851,8 +9040,11 @@
       <c r="G65" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I65" s="6">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>76</v>
       </c>
@@ -8874,8 +9066,11 @@
       <c r="G66" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I66" s="6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>72</v>
       </c>
@@ -8900,8 +9095,11 @@
       <c r="H67" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I67" s="6">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>73</v>
       </c>
@@ -8926,8 +9124,11 @@
       <c r="H68" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I68" s="6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>546</v>
       </c>
@@ -8952,8 +9153,11 @@
       <c r="H69" s="4" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I69" s="6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>225</v>
       </c>
@@ -8978,8 +9182,11 @@
       <c r="H70" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I70" s="6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>542</v>
       </c>
@@ -9004,8 +9211,11 @@
       <c r="H71" s="4" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I71" s="6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>218</v>
       </c>
@@ -9030,8 +9240,11 @@
       <c r="H72" s="4" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I72" s="6">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>548</v>
       </c>
@@ -9053,8 +9266,11 @@
       <c r="G73" s="4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I73" s="6">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>526</v>
       </c>
@@ -9079,8 +9295,11 @@
       <c r="H74" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I74" s="6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>538</v>
       </c>
@@ -9102,8 +9321,11 @@
       <c r="G75" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I75" s="6">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>236</v>
       </c>
@@ -9128,8 +9350,11 @@
       <c r="H76" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I76" s="6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>373</v>
       </c>
@@ -9154,8 +9379,11 @@
       <c r="H77" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I77" s="6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>74</v>
       </c>
@@ -9180,8 +9408,11 @@
       <c r="H78" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I78" s="6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>85</v>
       </c>
@@ -9206,8 +9437,11 @@
       <c r="H79" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I79" s="6">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>75</v>
       </c>
@@ -9232,8 +9466,11 @@
       <c r="H80" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I80" s="6">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>92</v>
       </c>
@@ -9255,8 +9492,11 @@
       <c r="G81" s="4" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I81" s="6">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>489</v>
       </c>
@@ -9281,8 +9521,11 @@
       <c r="H82" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I82" s="6">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>224</v>
       </c>
@@ -9307,8 +9550,11 @@
       <c r="H83" s="4" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I83" s="6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>93</v>
       </c>
@@ -9330,8 +9576,11 @@
       <c r="G84" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I84" s="6">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>94</v>
       </c>
@@ -9353,8 +9602,11 @@
       <c r="G85" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I85" s="6">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>230</v>
       </c>
@@ -9379,8 +9631,11 @@
       <c r="H86" s="4" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I86" s="6">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>231</v>
       </c>
@@ -9405,8 +9660,11 @@
       <c r="H87" s="4" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" ht="90" x14ac:dyDescent="0.35">
+      <c r="I87" s="6">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="90" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>95</v>
       </c>
@@ -9431,8 +9689,11 @@
       <c r="H88" s="4" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I88" s="6">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>100</v>
       </c>
@@ -9454,8 +9715,11 @@
       <c r="G89" s="4" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I89" s="6">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>232</v>
       </c>
@@ -9480,8 +9744,11 @@
       <c r="H90" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I90" s="6">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>233</v>
       </c>
@@ -9506,8 +9773,11 @@
       <c r="H91" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I91" s="6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>96</v>
       </c>
@@ -9532,8 +9802,11 @@
       <c r="H92" s="4" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I92" s="6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>91</v>
       </c>
@@ -9555,8 +9828,11 @@
       <c r="G93" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I93" s="6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>235</v>
       </c>
@@ -9578,8 +9854,11 @@
       <c r="G94" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I94" s="6">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>97</v>
       </c>
@@ -9601,8 +9880,11 @@
       <c r="G95" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I95" s="6">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>98</v>
       </c>
@@ -9627,8 +9909,11 @@
       <c r="H96" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I96" s="6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>529</v>
       </c>
@@ -9650,8 +9935,11 @@
       <c r="H97" s="4" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I97" s="6">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>227</v>
       </c>
@@ -9676,8 +9964,11 @@
       <c r="H98" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I98" s="6">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>517</v>
       </c>
@@ -9702,8 +9993,11 @@
       <c r="H99" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I99" s="6">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>220</v>
       </c>
@@ -9725,8 +10019,11 @@
       <c r="G100" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I100" s="6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>550</v>
       </c>
@@ -9748,8 +10045,11 @@
       <c r="H101" s="4" t="s">
         <v>797</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I101" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>99</v>
       </c>
@@ -9771,8 +10071,11 @@
       <c r="G102" s="4" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I102" s="6">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>240</v>
       </c>
@@ -9794,8 +10097,11 @@
       <c r="G103" s="4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I103" s="6">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>90</v>
       </c>
@@ -9817,8 +10123,11 @@
       <c r="G104" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I104" s="6">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>468</v>
       </c>
@@ -9843,8 +10152,11 @@
       <c r="H105" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I105" s="6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>364</v>
       </c>
@@ -9869,8 +10181,11 @@
       <c r="H106" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I106" s="6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>121</v>
       </c>
@@ -9895,8 +10210,11 @@
       <c r="H107" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I107" s="6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>122</v>
       </c>
@@ -9921,8 +10239,11 @@
       <c r="H108" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I108" s="6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>123</v>
       </c>
@@ -9947,8 +10268,11 @@
       <c r="H109" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I109" s="6">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>469</v>
       </c>
@@ -9970,8 +10294,11 @@
       <c r="G110" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I110" s="6">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>124</v>
       </c>
@@ -9996,8 +10323,11 @@
       <c r="H111" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I111" s="6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>125</v>
       </c>
@@ -10019,8 +10349,11 @@
       <c r="G112" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I112" s="6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>136</v>
       </c>
@@ -10045,8 +10378,11 @@
       <c r="H113" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I113" s="6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>139</v>
       </c>
@@ -10068,8 +10404,11 @@
       <c r="G114" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I114" s="6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>473</v>
       </c>
@@ -10094,8 +10433,11 @@
       <c r="H115" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I115" s="6">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>555</v>
       </c>
@@ -10117,8 +10459,11 @@
       <c r="G116" s="4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I116" s="6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>221</v>
       </c>
@@ -10143,8 +10488,11 @@
       <c r="H117" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I117" s="6">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>126</v>
       </c>
@@ -10166,8 +10514,11 @@
       <c r="G118" s="4" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I118" s="6">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>503</v>
       </c>
@@ -10189,8 +10540,11 @@
       <c r="G119" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I119" s="6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>535</v>
       </c>
@@ -10215,8 +10569,11 @@
       <c r="H120" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I120" s="6">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>540</v>
       </c>
@@ -10238,8 +10595,11 @@
       <c r="G121" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I121" s="6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>565</v>
       </c>
@@ -10264,8 +10624,11 @@
       <c r="H122" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I122" s="6">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>146</v>
       </c>
@@ -10290,8 +10653,11 @@
       <c r="H123" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I123" s="6">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>562</v>
       </c>
@@ -10310,8 +10676,11 @@
       <c r="G124" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.35">
+      <c r="I124" s="6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" s="8" customFormat="1" ht="54" x14ac:dyDescent="0.3">
       <c r="A125" s="5" t="s">
         <v>293</v>
       </c>
@@ -10336,8 +10705,11 @@
       <c r="H125" s="4" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I125" s="6">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
         <v>374</v>
       </c>
@@ -10359,8 +10731,11 @@
       <c r="H126" s="4" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I126" s="6">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
         <v>239</v>
       </c>
@@ -10385,8 +10760,11 @@
       <c r="H127" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" ht="108" x14ac:dyDescent="0.35">
+      <c r="I127" s="6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" ht="108" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
         <v>161</v>
       </c>
@@ -10411,8 +10789,11 @@
       <c r="H128" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I128" s="6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
         <v>370</v>
       </c>
@@ -10437,8 +10818,11 @@
       <c r="H129" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" ht="54.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I129" s="6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>160</v>
       </c>
@@ -10463,8 +10847,11 @@
       <c r="H130" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I130" s="6">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>159</v>
       </c>
@@ -10489,8 +10876,11 @@
       <c r="H131" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I131" s="6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>222</v>
       </c>
@@ -10515,8 +10905,11 @@
       <c r="H132" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I132" s="6">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>449</v>
       </c>
@@ -10538,8 +10931,11 @@
       <c r="G133" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" ht="31.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I133" s="6">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>444</v>
       </c>
@@ -10564,8 +10960,11 @@
       <c r="H134" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I134" s="6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
         <v>158</v>
       </c>
@@ -10590,8 +10989,11 @@
       <c r="H135" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I135" s="6">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>292</v>
       </c>
@@ -10616,8 +11018,11 @@
       <c r="H136" s="4" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I136" s="6">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
         <v>567</v>
       </c>
@@ -10642,8 +11047,11 @@
       <c r="H137" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I137" s="6">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>354</v>
       </c>
@@ -10668,8 +11076,11 @@
       <c r="H138" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I138" s="6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
         <v>157</v>
       </c>
@@ -10694,8 +11105,11 @@
       <c r="H139" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I139" s="6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
         <v>476</v>
       </c>
@@ -10720,8 +11134,11 @@
       <c r="H140" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I140" s="6">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
         <v>410</v>
       </c>
@@ -10746,8 +11163,11 @@
       <c r="H141" s="4" t="s">
         <v>794</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I141" s="6">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
         <v>504</v>
       </c>
@@ -10772,8 +11192,11 @@
       <c r="H142" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I142" s="6">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
         <v>156</v>
       </c>
@@ -10798,8 +11221,11 @@
       <c r="H143" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I143" s="6">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>376</v>
       </c>
@@ -10824,8 +11250,11 @@
       <c r="H144" s="4" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I144" s="6">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
         <v>155</v>
       </c>
@@ -10850,8 +11279,11 @@
       <c r="H145" s="4" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I145" s="6">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A146" s="4" t="s">
         <v>488</v>
       </c>
@@ -10876,8 +11308,11 @@
       <c r="H146" s="4" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I146" s="6">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
         <v>514</v>
       </c>
@@ -10902,8 +11337,11 @@
       <c r="H147" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" ht="53.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I147" s="6">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
         <v>173</v>
       </c>
@@ -10928,8 +11366,11 @@
       <c r="H148" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I148" s="6">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
         <v>324</v>
       </c>
@@ -10954,8 +11395,11 @@
       <c r="H149" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" ht="72" x14ac:dyDescent="0.35">
+      <c r="I149" s="6">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
         <v>223</v>
       </c>
@@ -10980,8 +11424,11 @@
       <c r="H150" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I150" s="6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
         <v>499</v>
       </c>
@@ -11006,8 +11453,11 @@
       <c r="H151" s="4" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I151" s="6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
         <v>363</v>
       </c>
@@ -11029,8 +11479,11 @@
       <c r="H152" s="4" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I152" s="6">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
         <v>219</v>
       </c>
@@ -11055,8 +11508,11 @@
       <c r="H153" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I153" s="6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
         <v>153</v>
       </c>
@@ -11081,8 +11537,11 @@
       <c r="H154" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I154" s="6">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
         <v>154</v>
       </c>
@@ -11107,8 +11566,11 @@
       <c r="H155" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I155" s="6">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A156" s="4" t="s">
         <v>152</v>
       </c>
@@ -11130,8 +11592,11 @@
       <c r="G156" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I156" s="6">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A157" s="4" t="s">
         <v>151</v>
       </c>
@@ -11156,8 +11621,11 @@
       <c r="H157" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I157" s="6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="4" t="s">
         <v>150</v>
       </c>
@@ -11182,8 +11650,11 @@
       <c r="H158" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I158" s="6">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
         <v>509</v>
       </c>
@@ -11208,8 +11679,11 @@
       <c r="H159" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I159" s="6">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
         <v>149</v>
       </c>
@@ -11231,8 +11705,11 @@
       <c r="G160" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I160" s="6">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A161" s="4" t="s">
         <v>148</v>
       </c>
@@ -11254,8 +11731,11 @@
       <c r="G161" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I161" s="6">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" s="4" t="s">
         <v>520</v>
       </c>
@@ -11280,8 +11760,11 @@
       <c r="H162" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="I162" s="6">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A163" s="4" t="s">
         <v>393</v>
       </c>
@@ -11306,8 +11789,11 @@
       <c r="H163" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I163" s="6">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
         <v>147</v>
       </c>
@@ -11332,8 +11818,11 @@
       <c r="H164" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I164" s="6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="4" t="s">
         <v>229</v>
       </c>
@@ -11358,8 +11847,11 @@
       <c r="H165" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I165" s="6">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
         <v>390</v>
       </c>
@@ -11384,8 +11876,11 @@
       <c r="H166" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I166" s="6">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>197</v>
       </c>
@@ -11410,8 +11905,11 @@
       <c r="H167" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="I167" s="6">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
         <v>198</v>
       </c>
@@ -11436,8 +11934,11 @@
       <c r="H168" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I168" s="6">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
         <v>442</v>
       </c>
@@ -11459,8 +11960,11 @@
       <c r="H169" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I169" s="6">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A170" s="4" t="s">
         <v>372</v>
       </c>
@@ -11482,8 +11986,11 @@
       <c r="G170" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I170" s="6">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
         <v>199</v>
       </c>
@@ -11502,8 +12009,11 @@
       <c r="F171" s="7" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I171" s="6">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A172" s="4" t="s">
         <v>378</v>
       </c>
@@ -11528,8 +12038,11 @@
       <c r="H172" s="4" t="s">
         <v>796</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I172" s="6">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A173" s="4" t="s">
         <v>201</v>
       </c>
@@ -11554,8 +12067,11 @@
       <c r="H173" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I173" s="6">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A174" s="4" t="s">
         <v>294</v>
       </c>
@@ -11580,8 +12096,11 @@
       <c r="H174" s="4" t="s">
         <v>787</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I174" s="6">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A175" s="4" t="s">
         <v>202</v>
       </c>
@@ -11606,8 +12125,11 @@
       <c r="H175" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I175" s="6">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A176" s="4" t="s">
         <v>203</v>
       </c>
@@ -11629,8 +12151,11 @@
       <c r="G176" s="4" t="s">
         <v>799</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I176" s="6">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A177" s="4" t="s">
         <v>204</v>
       </c>
@@ -11655,8 +12180,11 @@
       <c r="H177" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I177" s="6">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A178" s="4" t="s">
         <v>321</v>
       </c>
@@ -11681,8 +12209,11 @@
       <c r="H178" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I178" s="6">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A179" s="4" t="s">
         <v>371</v>
       </c>
@@ -11704,8 +12235,11 @@
       <c r="G179" s="4" t="s">
         <v>800</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I179" s="6">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A180" s="4" t="s">
         <v>394</v>
       </c>
@@ -11730,8 +12264,11 @@
       <c r="H180" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I180" s="6">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A181" s="4" t="s">
         <v>242</v>
       </c>
@@ -11756,8 +12293,11 @@
       <c r="H181" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I181" s="6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A182" s="4" t="s">
         <v>205</v>
       </c>
@@ -11782,8 +12322,11 @@
       <c r="H182" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I182" s="6">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A183" s="4" t="s">
         <v>200</v>
       </c>
@@ -11805,8 +12348,11 @@
       <c r="H183" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I183" s="6">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" s="4" t="s">
         <v>350</v>
       </c>
@@ -11831,8 +12377,11 @@
       <c r="H184" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I184" s="6">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" s="4" t="s">
         <v>206</v>
       </c>
@@ -11857,8 +12406,11 @@
       <c r="H185" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+      <c r="I185" s="6">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A186" s="4" t="s">
         <v>216</v>
       </c>
@@ -11883,8 +12435,11 @@
       <c r="H186" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I186" s="6">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A187" s="4" t="s">
         <v>217</v>
       </c>
@@ -11909,8 +12464,11 @@
       <c r="H187" s="4" t="s">
         <v>793</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I187" s="6">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A188" s="4" t="s">
         <v>207</v>
       </c>
@@ -11935,8 +12493,11 @@
       <c r="H188" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I188" s="6">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" s="4" t="s">
         <v>417</v>
       </c>
@@ -11961,8 +12522,11 @@
       <c r="H189" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I189" s="6">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="5" t="s">
         <v>208</v>
       </c>
@@ -11987,8 +12551,11 @@
       <c r="H190" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I190" s="6">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" s="4" t="s">
         <v>558</v>
       </c>
@@ -12007,8 +12574,11 @@
       <c r="G191" s="4" t="s">
         <v>803</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I191" s="6">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
         <v>243</v>
       </c>
@@ -12033,8 +12603,11 @@
       <c r="H192" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I192" s="6">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
         <v>210</v>
       </c>
@@ -12059,8 +12632,11 @@
       <c r="H193" s="4" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I193" s="6">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
         <v>209</v>
       </c>
@@ -12085,8 +12661,11 @@
       <c r="H194" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I194" s="6">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
         <v>211</v>
       </c>
@@ -12111,8 +12690,11 @@
       <c r="H195" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I195" s="6">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
         <v>212</v>
       </c>
@@ -12137,8 +12719,11 @@
       <c r="H196" s="4" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="I196" s="6">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
         <v>234</v>
       </c>
@@ -12163,8 +12748,11 @@
       <c r="H197" s="4" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I197" s="6">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A198" s="4" t="s">
         <v>226</v>
       </c>
@@ -12189,8 +12777,11 @@
       <c r="H198" s="4" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I198" s="6">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199" s="4" t="s">
         <v>446</v>
       </c>
@@ -12215,8 +12806,11 @@
       <c r="H199" s="4" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I199" s="6">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A200" s="4" t="s">
         <v>213</v>
       </c>
@@ -12238,8 +12832,11 @@
       <c r="G200" s="4" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I200" s="6">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A201" s="4" t="s">
         <v>214</v>
       </c>
@@ -12264,8 +12861,11 @@
       <c r="H201" s="4" t="s">
         <v>790</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I201" s="6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A202" s="4" t="s">
         <v>215</v>
       </c>
@@ -12290,8 +12890,11 @@
       <c r="H202" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+      <c r="I202" s="6">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A203" s="4" t="s">
         <v>511</v>
       </c>
@@ -12316,8 +12919,11 @@
       <c r="H203" s="4" t="s">
         <v>791</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" ht="52.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I203" s="6">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="4" t="s">
         <v>196</v>
       </c>
@@ -12341,6 +12947,9 @@
       </c>
       <c r="H204" s="4" t="s">
         <v>785</v>
+      </c>
+      <c r="I204" s="6">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -12560,1007 +13169,1007 @@
       <selection sqref="A1:A200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.453125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="65.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="87" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="130" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="161" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="164" spans="1:1" ht="58" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="165" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="173" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="181" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="186" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="200" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>281</v>
       </c>

</xml_diff>